<commit_message>
primary changes into page
</commit_message>
<xml_diff>
--- a/Filter.xlsx
+++ b/Filter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10056" windowHeight="4548" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="عملگرها" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="428">
   <si>
     <t>توضیح</t>
   </si>
@@ -1240,6 +1240,75 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>تعداد خرید حقیقی</t>
+  </si>
+  <si>
+    <t>تعداد فروش حقیقی</t>
+  </si>
+  <si>
+    <t>حجم فروش حقیقی</t>
+  </si>
+  <si>
+    <t>تعداد خرید حقوقی</t>
+  </si>
+  <si>
+    <t>حجم فروش حقوقی</t>
+  </si>
+  <si>
+    <t>تعداد فروش حقوقی</t>
+  </si>
+  <si>
+    <t>حچم مبنا</t>
+  </si>
+  <si>
+    <t>حجم شناور</t>
+  </si>
+  <si>
+    <t>e0</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>e9</t>
+  </si>
+  <si>
+    <t>میانگین حچم ماه</t>
+  </si>
+  <si>
+    <t>document.querySelector("#TopBox &gt; div.box2.zi1 &gt; div:nth-child(4) &gt; table &gt; tbody &gt; tr:nth-child(4) &gt; td:nth-child(2) &gt; div").getAttribute('title')</t>
+  </si>
+  <si>
+    <t>document.querySelector("#TopBox &gt; div.box2.zi1 &gt; div:nth-child(4) &gt; table &gt; tbody &gt; tr:nth-child(3) &gt; td:nth-child(2)").textContent</t>
+  </si>
+  <si>
+    <t>document.querySelector("#TopBox &gt; div.box2.zi1 &gt; div:nth-child(4) &gt; table &gt; tbody &gt; tr:nth-child(2) &gt; td:nth-child(2) &gt; div").getAttribute('title')</t>
+  </si>
+  <si>
+    <t>d08</t>
+  </si>
+  <si>
+    <t>document.querySelector("#d09 &gt; div").getAttribute('title')</t>
+  </si>
+  <si>
+    <t>document.querySelector("#d10 &gt; div").getAttribute('title')</t>
   </si>
 </sst>
 </file>
@@ -1591,6 +1660,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1609,10 +1684,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1626,18 +1707,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2010,19 +2079,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="24.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="42" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -2033,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A3" s="34" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A4" s="34" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A5" s="34" t="s">
         <v>11</v>
       </c>
@@ -2077,7 +2146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
@@ -2088,7 +2157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A7" s="34" t="s">
         <v>17</v>
       </c>
@@ -2099,7 +2168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
@@ -2110,7 +2179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A9" s="34" t="s">
         <v>23</v>
       </c>
@@ -2121,7 +2190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A10" s="34" t="s">
         <v>26</v>
       </c>
@@ -2132,7 +2201,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A11" s="34" t="s">
         <v>29</v>
       </c>
@@ -2143,7 +2212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A12" s="34" t="s">
         <v>31</v>
       </c>
@@ -2154,7 +2223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A13" s="34" t="s">
         <v>34</v>
       </c>
@@ -2165,7 +2234,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A14" s="34" t="s">
         <v>37</v>
       </c>
@@ -2176,7 +2245,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A15" s="34" t="s">
         <v>40</v>
       </c>
@@ -2187,212 +2256,212 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
     </row>
-    <row r="18" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
     </row>
-    <row r="19" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A19" s="35"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
     </row>
-    <row r="20" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A20" s="35"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
     </row>
-    <row r="21" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
     </row>
-    <row r="22" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
     </row>
-    <row r="23" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A23" s="35"/>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
     </row>
-    <row r="24" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A24" s="35"/>
       <c r="B24" s="35"/>
       <c r="C24" s="35"/>
     </row>
-    <row r="25" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
     </row>
-    <row r="26" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A26" s="35"/>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
     </row>
-    <row r="27" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A27" s="35"/>
       <c r="B27" s="35"/>
       <c r="C27" s="35"/>
     </row>
-    <row r="28" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A28" s="35"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
     </row>
-    <row r="29" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A29" s="35"/>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
     </row>
-    <row r="30" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A30" s="35"/>
       <c r="B30" s="35"/>
       <c r="C30" s="35"/>
     </row>
-    <row r="31" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A31" s="35"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
     </row>
-    <row r="32" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A32" s="35"/>
       <c r="B32" s="35"/>
       <c r="C32" s="35"/>
     </row>
-    <row r="33" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A33" s="35"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
     </row>
-    <row r="34" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A34" s="35"/>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
     </row>
-    <row r="35" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A35" s="35"/>
       <c r="B35" s="35"/>
       <c r="C35" s="35"/>
     </row>
-    <row r="36" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A36" s="35"/>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
     </row>
-    <row r="37" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A37" s="35"/>
       <c r="B37" s="35"/>
       <c r="C37" s="35"/>
     </row>
-    <row r="38" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A38" s="35"/>
       <c r="B38" s="35"/>
       <c r="C38" s="35"/>
     </row>
-    <row r="39" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A39" s="35"/>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
     </row>
-    <row r="40" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A40" s="35"/>
       <c r="B40" s="35"/>
       <c r="C40" s="35"/>
     </row>
-    <row r="41" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A41" s="35"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35"/>
     </row>
-    <row r="42" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A42" s="35"/>
       <c r="B42" s="35"/>
       <c r="C42" s="35"/>
     </row>
-    <row r="43" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A43" s="35"/>
       <c r="B43" s="35"/>
       <c r="C43" s="35"/>
     </row>
-    <row r="44" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A44" s="35"/>
       <c r="B44" s="35"/>
       <c r="C44" s="35"/>
     </row>
-    <row r="45" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A45" s="35"/>
       <c r="B45" s="35"/>
       <c r="C45" s="35"/>
     </row>
-    <row r="46" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A46" s="35"/>
       <c r="B46" s="35"/>
       <c r="C46" s="35"/>
     </row>
-    <row r="47" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A47" s="35"/>
       <c r="B47" s="35"/>
       <c r="C47" s="35"/>
     </row>
-    <row r="48" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A48" s="35"/>
       <c r="B48" s="35"/>
       <c r="C48" s="35"/>
     </row>
-    <row r="49" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A49" s="35"/>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
     </row>
-    <row r="50" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A50" s="35"/>
       <c r="B50" s="35"/>
       <c r="C50" s="35"/>
     </row>
-    <row r="51" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A51" s="35"/>
       <c r="B51" s="35"/>
       <c r="C51" s="35"/>
     </row>
-    <row r="52" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A52" s="35"/>
       <c r="B52" s="35"/>
       <c r="C52" s="35"/>
     </row>
-    <row r="53" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A53" s="35"/>
       <c r="B53" s="35"/>
       <c r="C53" s="35"/>
     </row>
-    <row r="54" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A54" s="35"/>
       <c r="B54" s="35"/>
       <c r="C54" s="35"/>
     </row>
-    <row r="55" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A55" s="35"/>
       <c r="B55" s="35"/>
       <c r="C55" s="35"/>
     </row>
-    <row r="56" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A56" s="35"/>
       <c r="B56" s="35"/>
       <c r="C56" s="35"/>
     </row>
-    <row r="57" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
       <c r="A57" s="35"/>
       <c r="B57" s="35"/>
       <c r="C57" s="35"/>
@@ -2411,13 +2480,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2425,7 +2494,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -2433,7 +2502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -2441,7 +2510,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -2449,7 +2518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2457,7 +2526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -2465,7 +2534,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2473,7 +2542,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
@@ -2481,7 +2550,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
@@ -2489,7 +2558,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -2497,7 +2566,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
@@ -2519,15 +2588,15 @@
       <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="30.6" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="120.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="41.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="120.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2538,371 +2607,371 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A2" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A3" s="37"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="42" t="s">
+    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A3" s="39"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A4" s="38"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="43"/>
-    </row>
-    <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="36"/>
-      <c r="B5" s="39"/>
+    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="40"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A5" s="38"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A6" s="37"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="42" t="s">
+    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
-    </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="36" t="s">
+    <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="37"/>
+    </row>
+    <row r="8" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A8" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A9" s="37"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="42" t="s">
+    <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A9" s="39"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
-    </row>
-    <row r="11" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="36" t="s">
+    <row r="10" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="37"/>
+    </row>
+    <row r="11" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A11" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="41" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="42" t="s">
+    <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A12" s="39"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A13" s="38"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="43"/>
-    </row>
-    <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="36" t="s">
+    <row r="13" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A13" s="40"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="37"/>
+    </row>
+    <row r="14" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A14" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="41" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A15" s="37"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="42" t="s">
+    <row r="15" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="36" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="38"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="43"/>
-    </row>
-    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="36" t="s">
+    <row r="16" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="37"/>
+    </row>
+    <row r="17" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A17" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A18" s="37"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="42" t="s">
+    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A18" s="39"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A19" s="38"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
-    </row>
-    <row r="20" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="36" t="s">
+    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A19" s="40"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A20" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A21" s="37"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="42" t="s">
+    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A21" s="39"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="36" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A22" s="38"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="43"/>
-    </row>
-    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="36" t="s">
+    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="40"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="37"/>
+    </row>
+    <row r="23" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A23" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="41" t="s">
         <v>91</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A24" s="37"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="42" t="s">
+    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A24" s="39"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="36" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A25" s="38"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="43"/>
-    </row>
-    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="36" t="s">
+    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A25" s="40"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A26" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="41" t="s">
         <v>95</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A27" s="37"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="42" t="s">
+    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A27" s="39"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A28" s="38"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="43"/>
-    </row>
-    <row r="29" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="36" t="s">
+    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A28" s="40"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="37"/>
+    </row>
+    <row r="29" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A29" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="41" t="s">
         <v>99</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A30" s="37"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="42" t="s">
+    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A30" s="39"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="36" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A31" s="38"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="43"/>
-    </row>
-    <row r="32" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="36" t="s">
+    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="37"/>
+    </row>
+    <row r="32" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A32" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="41" t="s">
         <v>103</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A33" s="37"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="42" t="s">
+    <row r="33" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A33" s="39"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A34" s="38"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="43"/>
-    </row>
-    <row r="35" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="36" t="s">
+    <row r="34" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="37"/>
+    </row>
+    <row r="35" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A35" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="41" t="s">
         <v>107</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A36" s="37"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="42" t="s">
+    <row r="36" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A36" s="39"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A37" s="38"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="43"/>
-    </row>
-    <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="36" t="s">
+    <row r="37" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A37" s="40"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="37"/>
+    </row>
+    <row r="38" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A38" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="41" t="s">
         <v>111</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="37"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="42" t="s">
+    <row r="39" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="39"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="38"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="43"/>
-    </row>
-    <row r="41" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="36" t="s">
+    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="40"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="37"/>
+    </row>
+    <row r="41" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A41" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="41" t="s">
         <v>115</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A42" s="37"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="42" t="s">
+    <row r="42" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A42" s="39"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A43" s="38"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="43"/>
-    </row>
-    <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="36" t="s">
+    <row r="43" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A43" s="40"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="37"/>
+    </row>
+    <row r="44" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A44" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="41" t="s">
         <v>117</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A45" s="37"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="42" t="s">
+    <row r="45" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A45" s="39"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="36" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A46" s="38"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="43"/>
-    </row>
-    <row r="47" spans="1:3" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="36" t="s">
+    <row r="46" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A46" s="40"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="37"/>
+    </row>
+    <row r="47" spans="1:3" ht="25.2" x14ac:dyDescent="0.5">
+      <c r="A47" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="41" t="s">
         <v>121</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A48" s="37"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="42" t="s">
+    <row r="48" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A48" s="39"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="36" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A49" s="38"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="43"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="A49" s="40"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="37"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" s="7" t="s">
         <v>124</v>
       </c>
@@ -2911,7 +2980,7 @@
       </c>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="7" t="s">
         <v>126</v>
       </c>
@@ -2920,7 +2989,7 @@
       </c>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" s="7" t="s">
         <v>128</v>
       </c>
@@ -2929,7 +2998,7 @@
       </c>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" s="7" t="s">
         <v>130</v>
       </c>
@@ -2938,7 +3007,7 @@
       </c>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" s="7" t="s">
         <v>132</v>
       </c>
@@ -2947,7 +3016,7 @@
       </c>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="7" t="s">
         <v>134</v>
       </c>
@@ -2956,7 +3025,7 @@
       </c>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" s="7" t="s">
         <v>136</v>
       </c>
@@ -2965,7 +3034,7 @@
       </c>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" s="7" t="s">
         <v>138</v>
       </c>
@@ -2974,7 +3043,7 @@
       </c>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" s="7" t="s">
         <v>140</v>
       </c>
@@ -2983,7 +3052,7 @@
       </c>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" s="7" t="s">
         <v>142</v>
       </c>
@@ -2992,7 +3061,7 @@
       </c>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" s="7" t="s">
         <v>144</v>
       </c>
@@ -3001,7 +3070,7 @@
       </c>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A61" s="7" t="s">
         <v>146</v>
       </c>
@@ -3010,7 +3079,7 @@
       </c>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" s="7" t="s">
         <v>148</v>
       </c>
@@ -3019,7 +3088,7 @@
       </c>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" s="7" t="s">
         <v>150</v>
       </c>
@@ -3028,7 +3097,7 @@
       </c>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" s="7" t="s">
         <v>152</v>
       </c>
@@ -3037,7 +3106,7 @@
       </c>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A65" s="7" t="s">
         <v>154</v>
       </c>
@@ -3046,7 +3115,7 @@
       </c>
       <c r="C65" s="8"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" s="7" t="s">
         <v>156</v>
       </c>
@@ -3055,7 +3124,7 @@
       </c>
       <c r="C66" s="8"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" s="7" t="s">
         <v>158</v>
       </c>
@@ -3064,7 +3133,7 @@
       </c>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68" s="7" t="s">
         <v>160</v>
       </c>
@@ -3073,7 +3142,7 @@
       </c>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" s="7" t="s">
         <v>162</v>
       </c>
@@ -3082,7 +3151,7 @@
       </c>
       <c r="C69" s="8"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" s="7" t="s">
         <v>164</v>
       </c>
@@ -3091,7 +3160,7 @@
       </c>
       <c r="C70" s="8"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" s="7" t="s">
         <v>166</v>
       </c>
@@ -3100,7 +3169,7 @@
       </c>
       <c r="C71" s="8"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A72" s="7" t="s">
         <v>168</v>
       </c>
@@ -3109,7 +3178,7 @@
       </c>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73" s="7" t="s">
         <v>170</v>
       </c>
@@ -3118,7 +3187,7 @@
       </c>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" s="7" t="s">
         <v>172</v>
       </c>
@@ -3127,7 +3196,7 @@
       </c>
       <c r="C74" s="8"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" s="7" t="s">
         <v>174</v>
       </c>
@@ -3136,21 +3205,37 @@
       </c>
       <c r="C75" s="8"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A76" s="9"/>
       <c r="B76" s="15"/>
       <c r="C76" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="C3:C4"/>
@@ -3167,30 +3252,14 @@
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C42:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3205,15 +3274,15 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="19" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="35.44140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" style="19" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>209</v>
       </c>
@@ -3224,198 +3293,198 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="48" t="s">
         <v>178</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="39"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="44" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="50" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="44"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="44" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="51"/>
-    </row>
-    <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="40"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="45"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="48" t="s">
         <v>183</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="39"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="39" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="37"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="49" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="39"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="39"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="39"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="48"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="47"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="48" t="s">
         <v>188</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="45"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="39"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="46"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="40"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="47"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="48"/>
-    </row>
-    <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="C15" s="51"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="47"/>
+    </row>
+    <row r="17" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="47"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="48"/>
-    </row>
-    <row r="19" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="C17" s="51"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="40"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="47"/>
+    </row>
+    <row r="19" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="47"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="48"/>
-    </row>
-    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="C19" s="51"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="40"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="47"/>
+    </row>
+    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="47"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="48"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="C21" s="51"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="40"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="47"/>
+    </row>
+    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="48" t="s">
         <v>200</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="49" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="39"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="46" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="48"/>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="40"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="47"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="C26" s="47"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="49"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="48"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C26" s="51"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="39"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="46"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="40"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="47"/>
+    </row>
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>205</v>
       </c>
@@ -3424,7 +3493,7 @@
       </c>
       <c r="C29" s="20"/>
     </row>
-    <row r="30" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>207</v>
       </c>
@@ -3433,63 +3502,63 @@
       </c>
       <c r="C30" s="20"/>
     </row>
-    <row r="31" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="9"/>
     </row>
-    <row r="32" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="9"/>
     </row>
-    <row r="33" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="9"/>
     </row>
-    <row r="35" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="9"/>
     </row>
-    <row r="36" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="9"/>
     </row>
-    <row r="37" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="9"/>
     </row>
-    <row r="38" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="9"/>
     </row>
-    <row r="39" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3503,13 +3572,13 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>209</v>
       </c>
@@ -3517,7 +3586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
         <v>210</v>
       </c>
@@ -3525,11 +3594,11 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
       <c r="B3" s="55"/>
     </row>
-    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
         <v>212</v>
       </c>
@@ -3537,11 +3606,11 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="53"/>
       <c r="B5" s="55"/>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="52" t="s">
         <v>214</v>
       </c>
@@ -3549,11 +3618,11 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="53"/>
       <c r="B7" s="55"/>
     </row>
-    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>216</v>
       </c>
@@ -3561,11 +3630,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="53"/>
       <c r="B9" s="55"/>
     </row>
-    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="52" t="s">
         <v>218</v>
       </c>
@@ -3573,11 +3642,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="53"/>
       <c r="B11" s="55"/>
     </row>
-    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="52" t="s">
         <v>220</v>
       </c>
@@ -3585,11 +3654,11 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
       <c r="B13" s="55"/>
     </row>
-    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
         <v>222</v>
       </c>
@@ -3597,11 +3666,11 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="53"/>
       <c r="B15" s="55"/>
     </row>
-    <row r="16" spans="1:2" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>224</v>
       </c>
@@ -3611,12 +3680,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:A9"/>
@@ -3625,6 +3688,12 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3639,14 +3708,14 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="27.33203125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="72.109375" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>209</v>
       </c>
@@ -3654,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>403</v>
       </c>
@@ -3662,7 +3731,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>226</v>
       </c>
@@ -3670,7 +3739,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>228</v>
       </c>
@@ -3678,7 +3747,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>230</v>
       </c>
@@ -3686,7 +3755,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>232</v>
       </c>
@@ -3694,7 +3763,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>234</v>
       </c>
@@ -3702,7 +3771,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>236</v>
       </c>
@@ -3710,7 +3779,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>238</v>
       </c>
@@ -3718,7 +3787,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>240</v>
       </c>
@@ -3726,7 +3795,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>242</v>
       </c>
@@ -3734,7 +3803,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>244</v>
       </c>
@@ -3742,7 +3811,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>246</v>
       </c>
@@ -3750,7 +3819,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>248</v>
       </c>
@@ -3758,7 +3827,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>250</v>
       </c>
@@ -3766,7 +3835,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>252</v>
       </c>
@@ -3774,7 +3843,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>254</v>
       </c>
@@ -3782,7 +3851,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>256</v>
       </c>
@@ -3790,7 +3859,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>258</v>
       </c>
@@ -3798,7 +3867,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>260</v>
       </c>
@@ -3806,7 +3875,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>262</v>
       </c>
@@ -3814,7 +3883,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>264</v>
       </c>
@@ -3822,7 +3891,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>266</v>
       </c>
@@ -3830,7 +3899,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>268</v>
       </c>
@@ -3838,7 +3907,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>270</v>
       </c>
@@ -3846,7 +3915,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>272</v>
       </c>
@@ -3854,7 +3923,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>274</v>
       </c>
@@ -3862,7 +3931,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>276</v>
       </c>
@@ -3870,7 +3939,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>278</v>
       </c>
@@ -3878,7 +3947,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>280</v>
       </c>
@@ -3886,7 +3955,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>282</v>
       </c>
@@ -3894,7 +3963,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>284</v>
       </c>
@@ -3902,7 +3971,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>286</v>
       </c>
@@ -3910,7 +3979,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>288</v>
       </c>
@@ -3918,7 +3987,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>290</v>
       </c>
@@ -3926,7 +3995,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>292</v>
       </c>
@@ -3934,7 +4003,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>294</v>
       </c>
@@ -3942,7 +4011,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>296</v>
       </c>
@@ -3950,7 +4019,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>297</v>
       </c>
@@ -3958,7 +4027,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>298</v>
       </c>
@@ -3966,7 +4035,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>299</v>
       </c>
@@ -3974,7 +4043,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>300</v>
       </c>
@@ -3982,7 +4051,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
         <v>301</v>
       </c>
@@ -3990,7 +4059,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
         <v>302</v>
       </c>
@@ -3998,7 +4067,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="27" t="s">
         <v>303</v>
       </c>
@@ -4006,7 +4075,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>304</v>
       </c>
@@ -4014,7 +4083,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
         <v>305</v>
       </c>
@@ -4022,7 +4091,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
         <v>306</v>
       </c>
@@ -4030,7 +4099,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
         <v>307</v>
       </c>
@@ -4038,7 +4107,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>308</v>
       </c>
@@ -4046,7 +4115,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
         <v>309</v>
       </c>
@@ -4054,7 +4123,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>310</v>
       </c>
@@ -4062,7 +4131,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>311</v>
       </c>
@@ -4070,7 +4139,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
         <v>312</v>
       </c>
@@ -4078,7 +4147,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="27" t="s">
         <v>313</v>
       </c>
@@ -4086,7 +4155,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
         <v>314</v>
       </c>
@@ -4094,7 +4163,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="27" t="s">
         <v>315</v>
       </c>
@@ -4102,7 +4171,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
         <v>316</v>
       </c>
@@ -4110,7 +4179,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
         <v>317</v>
       </c>
@@ -4118,7 +4187,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
         <v>318</v>
       </c>
@@ -4126,7 +4195,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
         <v>319</v>
       </c>
@@ -4134,7 +4203,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
         <v>320</v>
       </c>
@@ -4142,7 +4211,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
         <v>321</v>
       </c>
@@ -4150,7 +4219,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="27" t="s">
         <v>322</v>
       </c>
@@ -4158,7 +4227,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
         <v>323</v>
       </c>
@@ -4166,7 +4235,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
         <v>324</v>
       </c>
@@ -4174,7 +4243,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="27" t="s">
         <v>325</v>
       </c>
@@ -4182,7 +4251,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="27" t="s">
         <v>326</v>
       </c>
@@ -4190,7 +4259,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
         <v>317</v>
       </c>
@@ -4198,7 +4267,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
         <v>327</v>
       </c>
@@ -4206,7 +4275,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="27" t="s">
         <v>328</v>
       </c>
@@ -4214,7 +4283,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="27" t="s">
         <v>329</v>
       </c>
@@ -4222,7 +4291,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="27" t="s">
         <v>330</v>
       </c>
@@ -4230,7 +4299,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="27" t="s">
         <v>331</v>
       </c>
@@ -4238,7 +4307,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="27" t="s">
         <v>332</v>
       </c>
@@ -4246,7 +4315,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
         <v>333</v>
       </c>
@@ -4254,7 +4323,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="27" t="s">
         <v>334</v>
       </c>
@@ -4262,7 +4331,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="27" t="s">
         <v>335</v>
       </c>
@@ -4270,7 +4339,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="27" t="s">
         <v>336</v>
       </c>
@@ -4278,7 +4347,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="27" t="s">
         <v>337</v>
       </c>
@@ -4286,7 +4355,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="27" t="s">
         <v>338</v>
       </c>
@@ -4294,7 +4363,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
         <v>339</v>
       </c>
@@ -4302,7 +4371,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="27" t="s">
         <v>340</v>
       </c>
@@ -4310,7 +4379,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="27" t="s">
         <v>341</v>
       </c>
@@ -4318,7 +4387,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="27" t="s">
         <v>342</v>
       </c>
@@ -4326,7 +4395,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="27" t="s">
         <v>343</v>
       </c>
@@ -4334,7 +4403,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="27" t="s">
         <v>344</v>
       </c>
@@ -4342,7 +4411,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="27" t="s">
         <v>345</v>
       </c>
@@ -4350,7 +4419,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="27" t="s">
         <v>346</v>
       </c>
@@ -4358,7 +4427,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="27" t="s">
         <v>347</v>
       </c>
@@ -4366,7 +4435,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="27" t="s">
         <v>348</v>
       </c>
@@ -4374,163 +4443,163 @@
         <v>402</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="24"/>
     </row>
-    <row r="93" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="24"/>
     </row>
-    <row r="94" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="24"/>
     </row>
-    <row r="95" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="24"/>
     </row>
-    <row r="96" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="24"/>
     </row>
-    <row r="97" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="24"/>
     </row>
-    <row r="98" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="24"/>
     </row>
-    <row r="99" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="24"/>
     </row>
-    <row r="100" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="24"/>
     </row>
-    <row r="101" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="24"/>
     </row>
-    <row r="102" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="24"/>
     </row>
-    <row r="103" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="24"/>
     </row>
-    <row r="104" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="24"/>
     </row>
-    <row r="105" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="24"/>
     </row>
-    <row r="106" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="24"/>
     </row>
-    <row r="107" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="24"/>
     </row>
-    <row r="108" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="24"/>
     </row>
-    <row r="109" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="24"/>
     </row>
-    <row r="110" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="24"/>
     </row>
-    <row r="111" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="24"/>
     </row>
-    <row r="112" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="24"/>
     </row>
-    <row r="113" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="24"/>
     </row>
-    <row r="114" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="24"/>
     </row>
-    <row r="115" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="24"/>
     </row>
-    <row r="116" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="24"/>
     </row>
-    <row r="117" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="24"/>
     </row>
-    <row r="118" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="24"/>
     </row>
-    <row r="119" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="24"/>
     </row>
-    <row r="120" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="24"/>
     </row>
-    <row r="121" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="24"/>
     </row>
-    <row r="122" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="24"/>
     </row>
-    <row r="123" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="24"/>
     </row>
-    <row r="124" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="24"/>
     </row>
-    <row r="125" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="24"/>
     </row>
-    <row r="126" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="24"/>
     </row>
-    <row r="127" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="24"/>
     </row>
-    <row r="128" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="24"/>
     </row>
-    <row r="129" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="24"/>
     </row>
-    <row r="130" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="24"/>
     </row>
-    <row r="131" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B131" s="24"/>
     </row>
-    <row r="132" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="24"/>
     </row>
-    <row r="133" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="24"/>
     </row>
-    <row r="134" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="24"/>
     </row>
-    <row r="135" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="24"/>
     </row>
-    <row r="136" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="24"/>
     </row>
-    <row r="137" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="24"/>
     </row>
-    <row r="138" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B138" s="24"/>
     </row>
-    <row r="139" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="24"/>
     </row>
-    <row r="140" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="24"/>
     </row>
-    <row r="141" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="24"/>
     </row>
-    <row r="142" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="24"/>
     </row>
-    <row r="143" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="24"/>
     </row>
-    <row r="144" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="25"/>
     </row>
   </sheetData>
@@ -4544,12 +4613,131 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>412</v>
+      </c>
+      <c r="B13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B14" t="s">
+        <v>422</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>